<commit_message>
Sample + Time tests + Animator reading optimise
</commit_message>
<xml_diff>
--- a/Param Testing.xlsx
+++ b/Param Testing.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Time Step Params" sheetId="1" r:id="rId1"/>
+    <sheet name="Timing Characterisation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="23">
   <si>
     <t>N_water</t>
   </si>
@@ -67,14 +68,41 @@
   <si>
     <t>Num Density</t>
   </si>
+  <si>
+    <t>Time per step 1</t>
+  </si>
+  <si>
+    <t>Time per step 3</t>
+  </si>
+  <si>
+    <t>Time per step 2</t>
+  </si>
+  <si>
+    <t>Avg Time</t>
+  </si>
+  <si>
+    <t>milliseconds</t>
+  </si>
+  <si>
+    <t>Box Size</t>
+  </si>
+  <si>
+    <t>Ln Time</t>
+  </si>
+  <si>
+    <t>Ln N</t>
+  </si>
+  <si>
+    <t>TIME NOT COMPARABLE DUE TO DIFFERENT COMPUTER LOAD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -101,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -109,15 +137,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -243,7 +318,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$H$5:$H$11</c:f>
+                <c:f>'Time Step Params'!$H$5:$H$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
@@ -273,7 +348,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$H$5:$H$11</c:f>
+                <c:f>'Time Step Params'!$H$5:$H$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
@@ -317,7 +392,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$11</c:f>
+              <c:f>'Time Step Params'!$A$5:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -347,7 +422,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$5:$I$11</c:f>
+              <c:f>'Time Step Params'!$I$5:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -676,7 +751,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$H$17:$H$23</c:f>
+                <c:f>'Time Step Params'!$H$17:$H$23</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
@@ -706,7 +781,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$H$17:$H$23</c:f>
+                <c:f>'Time Step Params'!$H$17:$H$23</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
@@ -750,7 +825,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$23</c:f>
+              <c:f>'Time Step Params'!$A$17:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -780,7 +855,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$17:$I$23</c:f>
+              <c:f>'Time Step Params'!$I$17:$I$23</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1104,7 +1179,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$H$34:$H$40</c:f>
+                <c:f>'Time Step Params'!$H$34:$H$40</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
@@ -1134,7 +1209,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$H$34:$H$40</c:f>
+                <c:f>'Time Step Params'!$H$34:$H$40</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
@@ -1178,7 +1253,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$40</c:f>
+              <c:f>'Time Step Params'!$A$34:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1208,7 +1283,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$34:$I$40</c:f>
+              <c:f>'Time Step Params'!$I$34:$I$40</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1537,7 +1612,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$H$46:$H$52</c:f>
+                <c:f>'Time Step Params'!$H$46:$H$52</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
@@ -1567,7 +1642,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$H$46:$H$52</c:f>
+                <c:f>'Time Step Params'!$H$46:$H$52</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
@@ -1611,7 +1686,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$46:$A$52</c:f>
+              <c:f>'Time Step Params'!$A$46:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1641,7 +1716,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$46:$I$52</c:f>
+              <c:f>'Time Step Params'!$I$46:$I$52</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1943,7 +2018,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$60</c:f>
+              <c:f>'Time Step Params'!$I$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1981,7 +2056,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$H$61:$H$70</c:f>
+                <c:f>'Time Step Params'!$H$61:$H$70</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="10"/>
@@ -2020,7 +2095,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$H$61:$H$70</c:f>
+                <c:f>'Time Step Params'!$H$61:$H$70</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="10"/>
@@ -2073,7 +2148,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$61:$C$70</c:f>
+              <c:f>'Time Step Params'!$C$61:$C$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2112,7 +2187,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$61:$I$70</c:f>
+              <c:f>'Time Step Params'!$I$61:$I$70</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2289,6 +2364,798 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="403987136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Timing Characterisation'!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ln Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.11698578302712161"/>
+                  <c:y val="-8.0421405657626135E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Timing Characterisation'!$I$5:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.912023005428146</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6051701859880918</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2983173665480363</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9914645471079817</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6846117276679271</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.3777589082278725</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0709060887878188</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.7640532693477624</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.4572004499077078</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Timing Characterisation'!$J$5:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.1704160207970933</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8645967931803213</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5543808868814177</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.255400599550573</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9587157334201284</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6343729377961864</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3321066897041112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.0783300801295637</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.8954060063009299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF9C-4FDB-8203-A2D556B05299}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="397515312"/>
+        <c:axId val="355874712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="397515312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="355874712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="355874712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397515312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Timing Characterisation'!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ln Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.9187007874015748E-2"/>
+                  <c:y val="-2.7799650043744531E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Timing Characterisation'!$I$20:$I$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.912023005428146</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6051701859880918</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2983173665480363</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9914645471079817</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6846117276679271</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.3777589082278725</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0709060887878188</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.7640532693477624</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.4572004499077078</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Timing Characterisation'!$J$20:$J$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.82709515306968417</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5665304114228238</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2972374866674503</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0657246453740261</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8430301339411947</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5925914037812312</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3278114417757392</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.068849880935284</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.8681790359689376</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-11B3-4F4F-B870-92874E6845E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="397515312"/>
+        <c:axId val="355874712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="397515312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="355874712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="355874712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397515312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2537,6 +3404,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4602,6 +5549,1038 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5276,6 +7255,73 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5541,8 +7587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7025,4 +9071,823 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.01</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <f>A2*B2</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>4.5</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5" s="7">
+        <f>(A5/C5)^(1/3)</f>
+        <v>2.3207944168063896</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.96</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.28</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.43</v>
+      </c>
+      <c r="G5" s="1">
+        <f>AVERAGE(D5:F5)</f>
+        <v>3.2233333333333332</v>
+      </c>
+      <c r="H5" s="1">
+        <f>_xlfn.STDEV.S(D5:F5)</f>
+        <v>0.24006943440041126</v>
+      </c>
+      <c r="I5">
+        <f>LN(A5)</f>
+        <v>3.912023005428146</v>
+      </c>
+      <c r="J5">
+        <f>LN(G5)</f>
+        <v>1.1704160207970933</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="B6" s="7">
+        <f t="shared" ref="B6:B14" si="0">(A6/C6)^(1/3)</f>
+        <v>2.9240177382128656</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6.56</v>
+      </c>
+      <c r="G6" s="1">
+        <f>AVERAGE(D6:F6)</f>
+        <v>6.4533333333333331</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" ref="H6:H11" si="1">_xlfn.STDEV.S(D6:F6)</f>
+        <v>9.2376043070339697E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I13" si="2">LN(A6)</f>
+        <v>4.6051701859880918</v>
+      </c>
+      <c r="J6">
+        <f>LN(G6)</f>
+        <v>1.8645967931803213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>200</v>
+      </c>
+      <c r="B7" s="7">
+        <f t="shared" si="0"/>
+        <v>3.6840314986403864</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>12.66</v>
+      </c>
+      <c r="E7" s="1">
+        <v>13.28</v>
+      </c>
+      <c r="F7" s="1">
+        <v>12.65</v>
+      </c>
+      <c r="G7" s="1">
+        <f>AVERAGE(D7:F7)</f>
+        <v>12.863333333333332</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.36087855759705778</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>5.2983173665480363</v>
+      </c>
+      <c r="J7">
+        <f>LN(G7)</f>
+        <v>2.5543808868814177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>400</v>
+      </c>
+      <c r="B8" s="7">
+        <f t="shared" si="0"/>
+        <v>4.6415888336127793</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>26.09</v>
+      </c>
+      <c r="E8" s="1">
+        <v>25.15</v>
+      </c>
+      <c r="F8" s="1">
+        <v>26.55</v>
+      </c>
+      <c r="G8" s="1">
+        <f>AVERAGE(D8:F8)</f>
+        <v>25.929999999999996</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.71358251099645198</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>5.9914645471079817</v>
+      </c>
+      <c r="J8">
+        <f>LN(G8)</f>
+        <v>3.255400599550573</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>800</v>
+      </c>
+      <c r="B9" s="7">
+        <f t="shared" si="0"/>
+        <v>5.8480354764257312</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>51.71</v>
+      </c>
+      <c r="E9" s="1">
+        <v>52.65</v>
+      </c>
+      <c r="F9" s="1">
+        <v>52.81</v>
+      </c>
+      <c r="G9" s="1">
+        <f>AVERAGE(D9:F9)</f>
+        <v>52.390000000000008</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.59430631832414504</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>6.6846117276679271</v>
+      </c>
+      <c r="J9">
+        <f>LN(G9)</f>
+        <v>3.9587157334201284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1600</v>
+      </c>
+      <c r="B10" s="7">
+        <f t="shared" si="0"/>
+        <v>7.3680629972807719</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>104.06</v>
+      </c>
+      <c r="E10" s="1">
+        <v>103.59</v>
+      </c>
+      <c r="F10" s="1">
+        <v>101.24</v>
+      </c>
+      <c r="G10" s="1">
+        <f>AVERAGE(D10:F10)</f>
+        <v>102.96333333333332</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5108386192222341</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>7.3777589082278725</v>
+      </c>
+      <c r="J10">
+        <f>LN(G10)</f>
+        <v>4.6343729377961864</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3200</v>
+      </c>
+      <c r="B11" s="7">
+        <f t="shared" si="0"/>
+        <v>9.283177667225555</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>206.24</v>
+      </c>
+      <c r="E11" s="1">
+        <v>208.91</v>
+      </c>
+      <c r="F11" s="1">
+        <v>205.47</v>
+      </c>
+      <c r="G11" s="1">
+        <f>AVERAGE(D11:F11)</f>
+        <v>206.87333333333333</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8053346873456242</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>8.0709060887878188</v>
+      </c>
+      <c r="J11">
+        <f>LN(G11)</f>
+        <v>5.3321066897041112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6400</v>
+      </c>
+      <c r="B12" s="7">
+        <f t="shared" si="0"/>
+        <v>11.696070952851464</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>432.96</v>
+      </c>
+      <c r="E12" s="1">
+        <v>433.28</v>
+      </c>
+      <c r="F12" s="1">
+        <v>442.66</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" ref="G12:G14" si="3">AVERAGE(D12:F12)</f>
+        <v>436.3</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" ref="H12:H14" si="4">_xlfn.STDEV.S(D12:F12)</f>
+        <v>5.5102450036273618</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>8.7640532693477624</v>
+      </c>
+      <c r="J12">
+        <f>LN(G12)</f>
+        <v>6.0783300801295637</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12800</v>
+      </c>
+      <c r="B13" s="7">
+        <f t="shared" si="0"/>
+        <v>14.736125994561549</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1">
+        <v>989.37</v>
+      </c>
+      <c r="E13" s="1">
+        <v>999.9</v>
+      </c>
+      <c r="F13" s="1">
+        <v>973.91</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="3"/>
+        <v>987.72666666666657</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="4"/>
+        <v>13.072698012779668</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>9.4572004499077078</v>
+      </c>
+      <c r="J13">
+        <f>LN(G13)</f>
+        <v>6.8954060063009299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>50</v>
+      </c>
+      <c r="B20" s="7">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <f>A20/B20^3</f>
+        <v>0.05</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="G20" s="1">
+        <f>AVERAGE(D20:F20)</f>
+        <v>2.2866666666666666</v>
+      </c>
+      <c r="H20" s="1">
+        <f>_xlfn.STDEV.S(D20:F20)</f>
+        <v>9.2376043070339947E-2</v>
+      </c>
+      <c r="I20">
+        <f>LN(A20)</f>
+        <v>3.912023005428146</v>
+      </c>
+      <c r="J20">
+        <f>LN(G20)</f>
+        <v>0.82709515306968417</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>100</v>
+      </c>
+      <c r="B21" s="7">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:C28" si="5">A21/B21^3</f>
+        <v>0.1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="E21" s="1">
+        <v>4.84</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4.84</v>
+      </c>
+      <c r="G21" s="1">
+        <f>AVERAGE(D21:F21)</f>
+        <v>4.79</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" ref="H21:H28" si="6">_xlfn.STDEV.S(D21:F21)</f>
+        <v>8.6602540378443546E-2</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ref="I21:I28" si="7">LN(A21)</f>
+        <v>4.6051701859880918</v>
+      </c>
+      <c r="J21">
+        <f>LN(G21)</f>
+        <v>1.5665304114228238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>200</v>
+      </c>
+      <c r="B22" s="7">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>9.84</v>
+      </c>
+      <c r="E22" s="1">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1">
+        <v>10</v>
+      </c>
+      <c r="G22" s="1">
+        <f>AVERAGE(D22:F22)</f>
+        <v>9.9466666666666672</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="6"/>
+        <v>9.2376043070340197E-2</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="7"/>
+        <v>5.2983173665480363</v>
+      </c>
+      <c r="J22">
+        <f>LN(G22)</f>
+        <v>2.2972374866674503</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>400</v>
+      </c>
+      <c r="B23" s="7">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="5"/>
+        <v>0.4</v>
+      </c>
+      <c r="D23" s="1">
+        <v>21.4</v>
+      </c>
+      <c r="E23" s="1">
+        <v>21.86</v>
+      </c>
+      <c r="F23" s="1">
+        <v>21.09</v>
+      </c>
+      <c r="G23" s="1">
+        <f>AVERAGE(D23:F23)</f>
+        <v>21.45</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="6"/>
+        <v>0.38742741255621022</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="7"/>
+        <v>5.9914645471079817</v>
+      </c>
+      <c r="J23">
+        <f>LN(G23)</f>
+        <v>3.0657246453740261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>800</v>
+      </c>
+      <c r="B24" s="7">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="D24" s="1">
+        <v>46.09</v>
+      </c>
+      <c r="E24" s="1">
+        <v>46.41</v>
+      </c>
+      <c r="F24" s="1">
+        <v>47.5</v>
+      </c>
+      <c r="G24" s="1">
+        <f>AVERAGE(D24:F24)</f>
+        <v>46.666666666666664</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="6"/>
+        <v>0.73921129140005171</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="7"/>
+        <v>6.6846117276679271</v>
+      </c>
+      <c r="J24">
+        <f>LN(G24)</f>
+        <v>3.8430301339411947</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1600</v>
+      </c>
+      <c r="B25" s="7">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="5"/>
+        <v>1.6</v>
+      </c>
+      <c r="D25" s="1">
+        <v>96.56</v>
+      </c>
+      <c r="E25" s="1">
+        <v>100.31</v>
+      </c>
+      <c r="F25" s="1">
+        <v>99.38</v>
+      </c>
+      <c r="G25" s="1">
+        <f>AVERAGE(D25:F25)</f>
+        <v>98.75</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="6"/>
+        <v>1.9527672672389804</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="7"/>
+        <v>7.3777589082278725</v>
+      </c>
+      <c r="J25">
+        <f>LN(G25)</f>
+        <v>4.5925914037812312</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3200</v>
+      </c>
+      <c r="B26" s="7">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="5"/>
+        <v>3.2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>203.59</v>
+      </c>
+      <c r="E26" s="1">
+        <v>207.96</v>
+      </c>
+      <c r="F26" s="1">
+        <v>206.41</v>
+      </c>
+      <c r="G26" s="1">
+        <f>AVERAGE(D26:F26)</f>
+        <v>205.98666666666668</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="6"/>
+        <v>2.2155435751375641</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="7"/>
+        <v>8.0709060887878188</v>
+      </c>
+      <c r="J26">
+        <f>LN(G26)</f>
+        <v>5.3278114417757392</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>6400</v>
+      </c>
+      <c r="B27" s="7">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="5"/>
+        <v>6.4</v>
+      </c>
+      <c r="D27" s="1">
+        <v>431.56</v>
+      </c>
+      <c r="E27" s="1">
+        <v>432.03</v>
+      </c>
+      <c r="F27" s="1">
+        <v>432.96</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" ref="G27:G28" si="8">AVERAGE(D27:F27)</f>
+        <v>432.18333333333334</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="6"/>
+        <v>0.71248391794714927</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="7"/>
+        <v>8.7640532693477624</v>
+      </c>
+      <c r="J27">
+        <f>LN(G27)</f>
+        <v>6.068849880935284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>12800</v>
+      </c>
+      <c r="B28" s="7">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="5"/>
+        <v>12.8</v>
+      </c>
+      <c r="D28" s="1">
+        <v>969.69</v>
+      </c>
+      <c r="E28" s="1">
+        <v>960.77</v>
+      </c>
+      <c r="F28" s="1">
+        <v>953.13</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="8"/>
+        <v>961.19666666666672</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="6"/>
+        <v>8.2882406657464909</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="7"/>
+        <v>9.4572004499077078</v>
+      </c>
+      <c r="J28">
+        <f>LN(G28)</f>
+        <v>6.8681790359689376</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D18:G18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>